<commit_message>
Update Day Two field mapping tools and add summary documentation
- Add mapping summary markdown files for all 7 objects
- Add generate_summary_md.py tool for creating summaries from Excel
- Add PACKAGE_EMAIL.md and PACKAGE_README.md for distribution
- Update all transformer modules with latest implementations
- Update mapping Excel files with refined field matches
- Update migration notebooks with execution outputs
- Update Claude agents with improved semantic matching logic
- Update MIGRATION_PROGRESS.md with comprehensive session notes
- Update .gitignore to exclude .vscode/ and Windows nul artifact

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/day-two/mappings/ES_Address__c_to_BBF_Location__c_mapping.xlsx
+++ b/day-two/mappings/ES_Address__c_to_BBF_Location__c_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjero\Documents\repos\python-repo\python_scripts\ES-to-BBF-migration\day-two\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD6663F9-DBCA-454B-AC7A-58F3B02441A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F814C-1352-4F69-9963-6D4BDE27DD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -17,7 +17,6 @@
     <sheet name="Picklist_Mapping" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Field_Mapping!$A$1:$J$43</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Picklist_Mapping!$A$1:$H$21</definedName>
   </definedNames>
   <calcPr calcId="0"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="493" uniqueCount="208">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="212">
   <si>
     <t>BBF_Field_API_Name</t>
   </si>
@@ -57,6 +56,15 @@
     <t>Notes</t>
   </si>
   <si>
+    <t>ES_Final_Field</t>
+  </si>
+  <si>
+    <t>Include_in_Migration</t>
+  </si>
+  <si>
+    <t>Business_Notes</t>
+  </si>
+  <si>
     <t>CLLICode_Last_Part__c</t>
   </si>
   <si>
@@ -78,6 +86,9 @@
     <t>ES does not have CLLI code component breakdown - would need to parse CLLI__c</t>
   </si>
   <si>
+    <t>TBD</t>
+  </si>
+  <si>
     <t>CLLICode__c</t>
   </si>
   <si>
@@ -102,6 +113,9 @@
     <t>Exact semantic match - CLLI code is standard telecom location identifier</t>
   </si>
   <si>
+    <t>Yes</t>
+  </si>
+  <si>
     <t>CVAddressId__c</t>
   </si>
   <si>
@@ -400,9 +414,6 @@
   </si>
   <si>
     <t>boolean</t>
-  </si>
-  <si>
-    <t>Yes</t>
   </si>
   <si>
     <t>ES does not have this control flag for manual naming</t>
@@ -655,7 +666,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -668,6 +679,14 @@
       <sz val="11"/>
       <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -729,7 +748,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -752,6 +771,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1056,12 +1081,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J43"/>
+  <dimension ref="A1:M43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" sqref="A1:J43"/>
+      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1076,9 +1101,12 @@
     <col min="8" max="8" width="17.44140625" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="101.77734375" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="35" customWidth="1"/>
+    <col min="12" max="12" width="20" customWidth="1"/>
+    <col min="13" max="13" width="40" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1109,1226 +1137,1448 @@
       <c r="J1" s="1" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="K1" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="L1" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="M1" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A2" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="K2" s="11"/>
+      <c r="L2" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M2" s="11"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>17</v>
+        <v>39</v>
       </c>
       <c r="B3" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I3" s="3" t="s">
-        <v>23</v>
-      </c>
       <c r="J3" s="3" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="K3" s="11"/>
+      <c r="L3" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M3" s="11"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A4" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="C4" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D4" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I4" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J4" s="2" t="s">
+      <c r="I4" s="3" t="s">
         <v>27</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A5" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B5" s="4" t="s">
+      <c r="J4" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="K4" s="11"/>
+      <c r="L4" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D5" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E5" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="G5" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H5" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I5" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J5" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M4" s="11"/>
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A5" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I5" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="K5" s="11"/>
+      <c r="L5" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M5" s="11"/>
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>34</v>
+        <v>55</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>36</v>
+        <v>57</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>37</v>
+        <v>58</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="H6" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I6" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+        <v>60</v>
+      </c>
+      <c r="K6" s="11"/>
+      <c r="L6" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M6" s="11"/>
+    </row>
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" s="3" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>40</v>
+        <v>58</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>41</v>
+        <v>23</v>
       </c>
       <c r="D7" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E7" s="3" t="s">
-        <v>42</v>
+        <v>57</v>
       </c>
       <c r="F7" s="3" t="s">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="G7" s="3" t="s">
-        <v>41</v>
+        <v>59</v>
       </c>
       <c r="H7" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I7" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J7" s="3" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+        <v>61</v>
+      </c>
+      <c r="K7" s="11"/>
+      <c r="L7" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M7" s="11"/>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>45</v>
+        <v>89</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>46</v>
+        <v>90</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D8" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>48</v>
+        <v>92</v>
       </c>
       <c r="G8" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I8" s="3" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+        <v>93</v>
+      </c>
+      <c r="K8" s="11"/>
+      <c r="L8" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M8" s="11"/>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>50</v>
+        <v>103</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>52</v>
+        <v>105</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>53</v>
+        <v>106</v>
       </c>
       <c r="G9" s="3" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="H9" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I9" s="3" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+        <v>107</v>
+      </c>
+      <c r="K9" s="11"/>
+      <c r="L9" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M9" s="11"/>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>52</v>
+        <v>119</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>53</v>
+        <v>120</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>52</v>
+        <v>121</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>53</v>
+        <v>122</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>54</v>
+        <v>23</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>22</v>
+        <v>26</v>
       </c>
       <c r="I10" s="3" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A11" s="2" t="s">
-        <v>57</v>
-      </c>
-      <c r="B11" s="2" t="s">
-        <v>58</v>
-      </c>
-      <c r="C11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D11" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
-      <c r="G11" s="2"/>
-      <c r="H11" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I11" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J11" s="2" t="s">
-        <v>59</v>
-      </c>
-    </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A12" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="B12" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="C12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E12" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G12" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H12" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I12" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J12" s="4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+        <v>123</v>
+      </c>
+      <c r="K10" s="11"/>
+      <c r="L10" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M10" s="11"/>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="G11" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="K11" s="11"/>
+      <c r="L11" s="11" t="s">
+        <v>29</v>
+      </c>
+      <c r="M11" s="11"/>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A12" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E12" s="2"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K12" s="11"/>
+      <c r="L12" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M12" s="11"/>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>65</v>
+        <v>83</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>66</v>
+        <v>84</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E13" s="2"/>
       <c r="F13" s="2"/>
       <c r="G13" s="2"/>
       <c r="H13" s="2" t="s">
-        <v>14</v>
+        <v>76</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+        <v>85</v>
+      </c>
+      <c r="K13" s="11"/>
+      <c r="L13" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="11"/>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" s="2" t="s">
-        <v>69</v>
+        <v>86</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>70</v>
+        <v>87</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E14" s="2"/>
       <c r="F14" s="2"/>
       <c r="G14" s="2"/>
       <c r="H14" s="2" t="s">
-        <v>71</v>
+        <v>76</v>
       </c>
       <c r="I14" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>88</v>
+      </c>
+      <c r="K14" s="11"/>
+      <c r="L14" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="11"/>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="2"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>102</v>
+      </c>
+      <c r="K15" s="11"/>
+      <c r="L15" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="11"/>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A16" s="2" t="s">
+        <v>162</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>110</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="K16" s="11"/>
+      <c r="L16" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M16" s="11"/>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A17" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="G17" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="K17" s="11"/>
+      <c r="L17" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M17" s="11"/>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>65</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F18" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H18" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I18" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J18" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="K18" s="11"/>
+      <c r="L18" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M18" s="11"/>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A19" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="F19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="G19" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H19" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J19" s="4" t="s">
+        <v>82</v>
+      </c>
+      <c r="K19" s="11"/>
+      <c r="L19" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M19" s="11"/>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A20" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>96</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>97</v>
+      </c>
+      <c r="F20" s="4" t="s">
+        <v>98</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I20" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J20" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K20" s="11"/>
+      <c r="L20" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M20" s="11"/>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A21" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F21" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H21" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I21" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J21" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="K21" s="11"/>
+      <c r="L21" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M21" s="11"/>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A22" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="F22" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I22" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>115</v>
+      </c>
+      <c r="K22" s="11"/>
+      <c r="L22" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M22" s="11"/>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A23" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H23" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I23" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>118</v>
+      </c>
+      <c r="K23" s="11"/>
+      <c r="L23" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M23" s="11"/>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A24" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>120</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="F24" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I24" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J24" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="K24" s="11"/>
+      <c r="L24" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M24" s="11"/>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A25" s="4" t="s">
+        <v>165</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="F25" s="4" t="s">
+        <v>111</v>
+      </c>
+      <c r="G25" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="H25" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I25" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="J25" s="4" t="s">
+        <v>167</v>
+      </c>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="11"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="4" t="s">
+        <v>174</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>175</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="F26" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G26" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="J26" s="4" t="s">
+        <v>176</v>
+      </c>
+      <c r="K26" s="11"/>
+      <c r="L26" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M26" s="11"/>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A27" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C27" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="J14" s="2" t="s">
-        <v>72</v>
-      </c>
-    </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A15" s="4" t="s">
-        <v>73</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>74</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D15" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E15" s="4" t="s">
-        <v>75</v>
-      </c>
-      <c r="F15" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="G15" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H15" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I15" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J15" s="4" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>78</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>79</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
-      <c r="G16" s="2"/>
-      <c r="H16" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A17" s="2" t="s">
-        <v>81</v>
-      </c>
-      <c r="B17" s="2" t="s">
-        <v>82</v>
-      </c>
-      <c r="C17" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
-      <c r="G17" s="2"/>
-      <c r="H17" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I17" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J17" s="2" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A18" s="3" t="s">
-        <v>84</v>
-      </c>
-      <c r="B18" s="3" t="s">
-        <v>85</v>
-      </c>
-      <c r="C18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D18" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E18" s="3" t="s">
-        <v>86</v>
-      </c>
-      <c r="F18" s="3" t="s">
-        <v>87</v>
-      </c>
-      <c r="G18" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H18" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I18" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J18" s="3" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A19" s="4" t="s">
-        <v>89</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>90</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>91</v>
-      </c>
-      <c r="D19" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E19" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="F19" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="G19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H19" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I19" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J19" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A20" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="B20" s="2" t="s">
-        <v>96</v>
-      </c>
-      <c r="C20" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="D20" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
-      <c r="G20" s="2"/>
-      <c r="H20" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I20" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J20" s="2" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>99</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>100</v>
-      </c>
-      <c r="F21" s="3" t="s">
-        <v>101</v>
-      </c>
-      <c r="G21" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I21" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="J21" s="3" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A22" s="4" t="s">
-        <v>103</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>104</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D22" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E22" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G22" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H22" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I22" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J22" s="4" t="s">
-        <v>107</v>
-      </c>
-    </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>108</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>109</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D23" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>62</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>63</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H23" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I23" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J23" s="4" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>112</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H24" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I24" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J24" s="4" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>114</v>
-      </c>
-      <c r="B25" s="3" t="s">
-        <v>115</v>
-      </c>
-      <c r="C25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D25" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E25" s="3" t="s">
-        <v>116</v>
-      </c>
-      <c r="F25" s="3" t="s">
-        <v>117</v>
-      </c>
-      <c r="G25" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H25" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I25" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J25" s="3" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A26" s="2" t="s">
-        <v>119</v>
-      </c>
-      <c r="B26" s="2" t="s">
-        <v>120</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
-      <c r="G26" s="2"/>
-      <c r="H26" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
-        <v>122</v>
-      </c>
-      <c r="B27" s="2" t="s">
-        <v>123</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>124</v>
-      </c>
       <c r="D27" s="2" t="s">
-        <v>125</v>
+        <v>16</v>
       </c>
       <c r="E27" s="2"/>
       <c r="F27" s="2"/>
       <c r="G27" s="2"/>
       <c r="H27" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I27" s="2" t="s">
-        <v>23</v>
+        <v>18</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>126</v>
-      </c>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+        <v>19</v>
+      </c>
+      <c r="K27" s="11"/>
+      <c r="L27" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M27" s="11"/>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" s="2" t="s">
-        <v>127</v>
+        <v>30</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>128</v>
+        <v>31</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E28" s="2"/>
       <c r="F28" s="2"/>
       <c r="G28" s="2"/>
       <c r="H28" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+        <v>32</v>
+      </c>
+      <c r="K28" s="11"/>
+      <c r="L28" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M28" s="11"/>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" s="2" t="s">
-        <v>130</v>
+        <v>62</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>131</v>
+        <v>63</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>91</v>
+        <v>23</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E29" s="2"/>
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+        <v>64</v>
+      </c>
+      <c r="K29" s="11"/>
+      <c r="L29" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="11"/>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" s="2" t="s">
-        <v>133</v>
+        <v>70</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>134</v>
+        <v>71</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>91</v>
+        <v>72</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E30" s="2"/>
       <c r="F30" s="2"/>
       <c r="G30" s="2"/>
       <c r="H30" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+        <v>73</v>
+      </c>
+      <c r="K30" s="11"/>
+      <c r="L30" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M30" s="11"/>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" s="2" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>91</v>
+        <v>15</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" s="2"/>
       <c r="G31" s="2"/>
       <c r="H31" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+        <v>126</v>
+      </c>
+      <c r="K31" s="11"/>
+      <c r="L31" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M31" s="11"/>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>54</v>
+        <v>129</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>13</v>
+        <v>29</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
       <c r="G32" s="2"/>
       <c r="H32" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+        <v>130</v>
+      </c>
+      <c r="K32" s="11"/>
+      <c r="L32" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M32" s="11"/>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>128</v>
+        <v>132</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>67</v>
+        <v>23</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E33" s="2"/>
       <c r="F33" s="2"/>
       <c r="G33" s="2"/>
       <c r="H33" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>143</v>
-      </c>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+        <v>133</v>
+      </c>
+      <c r="K33" s="11"/>
+      <c r="L33" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M33" s="11"/>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E34" s="2"/>
       <c r="F34" s="2"/>
       <c r="G34" s="2"/>
       <c r="H34" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>146</v>
-      </c>
-    </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A35" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="B35" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="C35" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D35" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="3" t="s">
-        <v>147</v>
-      </c>
-      <c r="F35" s="3" t="s">
-        <v>148</v>
-      </c>
-      <c r="G35" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="I35" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="J35" s="3" t="s">
-        <v>149</v>
-      </c>
-    </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A36" s="4" t="s">
-        <v>150</v>
-      </c>
-      <c r="B36" s="4" t="s">
-        <v>115</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D36" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E36" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="F36" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G36" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>151</v>
-      </c>
-    </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+        <v>136</v>
+      </c>
+      <c r="K34" s="11"/>
+      <c r="L34" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M34" s="11"/>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A35" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+      <c r="G35" s="2"/>
+      <c r="H35" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="K35" s="11"/>
+      <c r="L35" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M35" s="11"/>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A36" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>96</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+      <c r="G36" s="2"/>
+      <c r="H36" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>142</v>
+      </c>
+      <c r="K36" s="11"/>
+      <c r="L36" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M36" s="11"/>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>54</v>
+        <v>59</v>
       </c>
       <c r="D37" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
       <c r="G37" s="2"/>
       <c r="H37" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>15</v>
+        <v>27</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+        <v>145</v>
+      </c>
+      <c r="K37" s="11"/>
+      <c r="L37" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M37" s="11"/>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>156</v>
+        <v>132</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>67</v>
+        <v>72</v>
       </c>
       <c r="D38" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" s="2"/>
       <c r="G38" s="2"/>
       <c r="H38" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J38" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="K38" s="11"/>
+      <c r="L38" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M38" s="11"/>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A39" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+      <c r="G39" s="2"/>
+      <c r="H39" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="K39" s="11"/>
+      <c r="L39" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M39" s="11"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A40" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="B40" s="2" t="s">
         <v>157</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A39" s="2" t="s">
+      <c r="C40" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="D40" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+      <c r="G40" s="2"/>
+      <c r="H40" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I40" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J40" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="B39" s="2" t="s">
+      <c r="K40" s="11"/>
+      <c r="L40" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M40" s="11"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A41" s="2" t="s">
         <v>159</v>
       </c>
-      <c r="C39" s="2" t="s">
-        <v>67</v>
-      </c>
-      <c r="D39" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="2" t="s">
-        <v>105</v>
-      </c>
-      <c r="F39" s="2" t="s">
-        <v>106</v>
-      </c>
-      <c r="G39" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="H39" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="I39" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="J39" s="2" t="s">
+      <c r="B41" s="2" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A40" s="4" t="s">
-        <v>161</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>162</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D40" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="4" t="s">
-        <v>105</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="G40" s="4" t="s">
-        <v>54</v>
-      </c>
-      <c r="H40" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I40" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="J40" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A41" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="B41" s="2" t="s">
-        <v>165</v>
-      </c>
       <c r="C41" s="2" t="s">
-        <v>12</v>
+        <v>72</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E41" s="2"/>
       <c r="F41" s="2"/>
       <c r="G41" s="2"/>
       <c r="H41" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>166</v>
-      </c>
-    </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+        <v>161</v>
+      </c>
+      <c r="K41" s="11"/>
+      <c r="L41" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M41" s="11"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>168</v>
+        <v>169</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="E42" s="2"/>
       <c r="F42" s="2"/>
       <c r="G42" s="2"/>
       <c r="H42" s="2" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>23</v>
+        <v>27</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>169</v>
-      </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
-      <c r="A43" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="B43" s="4" t="s">
+      <c r="K42" s="11"/>
+      <c r="L42" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M42" s="11"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A43" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D43" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="E43" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F43" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="G43" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="H43" s="4" t="s">
-        <v>32</v>
-      </c>
-      <c r="I43" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="J43" s="4" t="s">
+      <c r="B43" s="2" t="s">
         <v>172</v>
       </c>
+      <c r="C43" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+      <c r="G43" s="2"/>
+      <c r="H43" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="K43" s="11"/>
+      <c r="L43" s="11" t="s">
+        <v>20</v>
+      </c>
+      <c r="M43" s="11"/>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M43">
+    <sortCondition ref="H1:H43"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
@@ -2356,65 +2606,65 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" s="5" t="s">
-        <v>173</v>
+        <v>177</v>
       </c>
       <c r="B1" s="5" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="D1" s="5" t="s">
-        <v>176</v>
+        <v>180</v>
       </c>
       <c r="E1" s="5" t="s">
         <v>9</v>
       </c>
       <c r="F1" s="5" t="s">
-        <v>177</v>
+        <v>181</v>
       </c>
       <c r="G1" s="6" t="s">
-        <v>178</v>
+        <v>182</v>
       </c>
       <c r="H1" s="6" t="s">
-        <v>179</v>
+        <v>183</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="7" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B2" s="7" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="C2" s="7" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>180</v>
+        <v>184</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>181</v>
+        <v>185</v>
       </c>
       <c r="F2" s="7"/>
       <c r="G2" s="8"/>
       <c r="H2" s="8"/>
     </row>
-    <row r="3" spans="1:8" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:8" ht="28.8" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B3" s="9" t="s">
-        <v>182</v>
+        <v>186</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D3" s="9" t="s">
-        <v>183</v>
+        <v>187</v>
       </c>
       <c r="E3" s="9" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="F3" s="9"/>
       <c r="G3" s="8"/>
@@ -2422,402 +2672,402 @@
     </row>
     <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" s="9" t="s">
-        <v>100</v>
+        <v>105</v>
       </c>
       <c r="B4" s="9" t="s">
-        <v>185</v>
+        <v>189</v>
       </c>
       <c r="C4" s="9" t="s">
-        <v>98</v>
+        <v>103</v>
       </c>
       <c r="D4" s="9" t="s">
-        <v>186</v>
+        <v>190</v>
       </c>
       <c r="E4" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F4" s="9" t="s">
-        <v>188</v>
+        <v>192</v>
       </c>
       <c r="G4" s="8"/>
       <c r="H4" s="8"/>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>189</v>
+        <v>193</v>
       </c>
       <c r="C5" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E5" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G5" s="8"/>
       <c r="H5" s="8"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B6" s="9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="C6" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D6" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E6" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F6" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G6" s="8"/>
       <c r="H6" s="8"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>193</v>
+        <v>197</v>
       </c>
       <c r="C7" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D7" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E7" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F7" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G7" s="8"/>
       <c r="H7" s="8"/>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B8" s="9" t="s">
+        <v>198</v>
+      </c>
+      <c r="C8" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D8" s="9" t="s">
         <v>194</v>
       </c>
-      <c r="C8" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D8" s="9" t="s">
-        <v>190</v>
-      </c>
       <c r="E8" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F8" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G8" s="8"/>
       <c r="H8" s="8"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B9" s="9" t="s">
+        <v>199</v>
+      </c>
+      <c r="C9" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="D9" s="9" t="s">
+        <v>194</v>
+      </c>
+      <c r="E9" s="9" t="s">
+        <v>191</v>
+      </c>
+      <c r="F9" s="9" t="s">
         <v>195</v>
-      </c>
-      <c r="C9" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="D9" s="9" t="s">
-        <v>190</v>
-      </c>
-      <c r="E9" s="9" t="s">
-        <v>187</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>191</v>
       </c>
       <c r="G9" s="8"/>
       <c r="H9" s="8"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B10" s="9" t="s">
-        <v>196</v>
+        <v>200</v>
       </c>
       <c r="C10" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D10" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E10" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F10" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G10" s="8"/>
       <c r="H10" s="8"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>197</v>
+        <v>201</v>
       </c>
       <c r="C11" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D11" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E11" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F11" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G11" s="8"/>
       <c r="H11" s="8"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B12" s="9" t="s">
-        <v>198</v>
+        <v>202</v>
       </c>
       <c r="C12" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D12" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E12" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F12" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G12" s="8"/>
       <c r="H12" s="8"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="C13" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D13" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E13" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F13" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G13" s="8"/>
       <c r="H13" s="8"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B14" s="9" t="s">
-        <v>200</v>
+        <v>204</v>
       </c>
       <c r="C14" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D14" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E14" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G14" s="8"/>
       <c r="H14" s="8"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>201</v>
+        <v>205</v>
       </c>
       <c r="C15" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D15" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E15" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G15" s="8"/>
       <c r="H15" s="8"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B16" s="9" t="s">
-        <v>202</v>
+        <v>206</v>
       </c>
       <c r="C16" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D16" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E16" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F16" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G16" s="8"/>
       <c r="H16" s="8"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A17" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>203</v>
+        <v>207</v>
       </c>
       <c r="C17" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D17" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E17" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F17" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G17" s="8"/>
       <c r="H17" s="8"/>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A18" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B18" s="9" t="s">
-        <v>204</v>
+        <v>208</v>
       </c>
       <c r="C18" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D18" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E18" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F18" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G18" s="8"/>
       <c r="H18" s="8"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A19" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>205</v>
+        <v>209</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D19" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E19" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F19" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G19" s="8"/>
       <c r="H19" s="8"/>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A20" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B20" s="9" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="C20" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D20" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E20" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F20" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G20" s="8"/>
       <c r="H20" s="8"/>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A21" s="9" t="s">
-        <v>105</v>
+        <v>110</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>207</v>
+        <v>211</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>111</v>
+        <v>116</v>
       </c>
       <c r="D21" s="9" t="s">
-        <v>190</v>
+        <v>194</v>
       </c>
       <c r="E21" s="9" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="F21" s="9" t="s">
-        <v>191</v>
+        <v>195</v>
       </c>
       <c r="G21" s="8"/>
       <c r="H21" s="8"/>
     </row>
   </sheetData>
-  <autoFilter ref="A1:H21" xr:uid="{00000000-0001-0000-0100-000000000000}"/>
+  <autoFilter ref="A1:H21" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Update BAN prep for full-scale UAT migration test
- Add active PA MARKET DECOM exclusion logic (Step 1.5)
- Only exclude BANs with ACTIVE PA DECOM orders
- Cancelled/Disconnected PA DECOM orders are OK
- Remove POC limits (BAN_LIMIT=0, MAX_ORDERS_PER_BAN=0)
- Add Excel sheet for excluded BANs with reasons
- Update documentation with exclusion logic examples
- Update Address to Location field mapping

Filtering logic:
- BAN excluded if: has order with Active status AND PA MARKET DECOM
- BAN eligible if: has active orders, no active PA DECOM
- Cancelled/Disconnected orders don't affect eligibility

Co-Authored-By: Claude Opus 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/day-two/mappings/ES_Address__c_to_BBF_Location__c_mapping.xlsx
+++ b/day-two/mappings/ES_Address__c_to_BBF_Location__c_mapping.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\vjero\Documents\repos\python-repo\python_scripts\ES-to-BBF-migration\day-two\mappings\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D8F814C-1352-4F69-9963-6D4BDE27DD39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9408390-AD57-430E-97FA-0E456594C14A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="2895" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="544" uniqueCount="219">
   <si>
     <t>BBF_Field_API_Name</t>
   </si>
@@ -660,6 +660,27 @@
   </si>
   <si>
     <t>Wisconsin Expansion</t>
+  </si>
+  <si>
+    <t xml:space="preserve">make sure they do not match/duplicate locations </t>
+  </si>
+  <si>
+    <t>Possible Duplicate</t>
+  </si>
+  <si>
+    <t>process after to fillin these</t>
+  </si>
+  <si>
+    <t>valdiation process if valid true if ES false needs revalidation</t>
+  </si>
+  <si>
+    <t>investigate to use ES DIM4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EVS </t>
+  </si>
+  <si>
+    <t>need new regions</t>
   </si>
 </sst>
 </file>
@@ -689,7 +710,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="6">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -720,6 +741,42 @@
         <bgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -748,7 +805,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -778,6 +835,27 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1081,12 +1159,12 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:M43"/>
+  <dimension ref="A1:M44"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="B1" sqref="B1"/>
-      <selection pane="bottomLeft" activeCell="H1" sqref="H1:H1048576"/>
+      <selection pane="bottomLeft" activeCell="M32" sqref="M32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1149,34 +1227,34 @@
     </row>
     <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" s="3" t="s">
-        <v>21</v>
+        <v>103</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>22</v>
+        <v>104</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>24</v>
+        <v>105</v>
       </c>
       <c r="F2" s="3" t="s">
-        <v>25</v>
+        <v>106</v>
       </c>
       <c r="G2" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H2" s="3" t="s">
         <v>26</v>
       </c>
       <c r="I2" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J2" s="3" t="s">
-        <v>28</v>
+        <v>107</v>
       </c>
       <c r="K2" s="11"/>
       <c r="L2" s="11" t="s">
@@ -1184,12 +1262,12 @@
       </c>
       <c r="M2" s="11"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:13" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="3" t="s">
-        <v>39</v>
+        <v>21</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>23</v>
@@ -1198,10 +1276,10 @@
         <v>16</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>42</v>
+        <v>25</v>
       </c>
       <c r="G3" s="3" t="s">
         <v>23</v>
@@ -1210,38 +1288,40 @@
         <v>26</v>
       </c>
       <c r="I3" s="3" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J3" s="3" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="M3" s="11"/>
+      <c r="M3" s="11" t="s">
+        <v>212</v>
+      </c>
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" s="3" t="s">
-        <v>44</v>
+        <v>151</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>45</v>
+        <v>152</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="D4" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="3" t="s">
-        <v>47</v>
+        <v>151</v>
       </c>
       <c r="F4" s="3" t="s">
-        <v>48</v>
+        <v>152</v>
       </c>
       <c r="G4" s="3" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
       <c r="H4" s="3" t="s">
         <v>26</v>
@@ -1250,7 +1330,7 @@
         <v>27</v>
       </c>
       <c r="J4" s="3" t="s">
-        <v>49</v>
+        <v>153</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11" t="s">
@@ -1260,10 +1340,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>23</v>
@@ -1272,10 +1352,10 @@
         <v>16</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="F5" s="3" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G5" s="3" t="s">
         <v>23</v>
@@ -1284,10 +1364,10 @@
         <v>26</v>
       </c>
       <c r="I5" s="3" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J5" s="3" t="s">
-        <v>54</v>
+        <v>43</v>
       </c>
       <c r="K5" s="11"/>
       <c r="L5" s="11" t="s">
@@ -1297,25 +1377,25 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" s="3" t="s">
-        <v>55</v>
+        <v>44</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="D6" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="F6" s="3" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="G6" s="3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="H6" s="3" t="s">
         <v>26</v>
@@ -1324,7 +1404,7 @@
         <v>27</v>
       </c>
       <c r="J6" s="3" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="K6" s="11"/>
       <c r="L6" s="11" t="s">
@@ -1333,48 +1413,48 @@
       <c r="M6" s="11"/>
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E7" s="3" t="s">
-        <v>57</v>
-      </c>
-      <c r="F7" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="G7" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="A7" s="12" t="s">
+        <v>89</v>
+      </c>
+      <c r="B7" s="12" t="s">
+        <v>90</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>91</v>
+      </c>
+      <c r="F7" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I7" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="J7" s="3" t="s">
-        <v>61</v>
-      </c>
-      <c r="K7" s="11"/>
-      <c r="L7" s="11" t="s">
+      <c r="I7" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>93</v>
+      </c>
+      <c r="K7" s="13"/>
+      <c r="L7" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M7" s="11"/>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M7" s="13"/>
+    </row>
+    <row r="8" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>90</v>
+        <v>51</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>23</v>
@@ -1383,10 +1463,10 @@
         <v>16</v>
       </c>
       <c r="E8" s="3" t="s">
-        <v>91</v>
+        <v>52</v>
       </c>
       <c r="F8" s="3" t="s">
-        <v>92</v>
+        <v>53</v>
       </c>
       <c r="G8" s="3" t="s">
         <v>23</v>
@@ -1398,7 +1478,7 @@
         <v>27</v>
       </c>
       <c r="J8" s="3" t="s">
-        <v>93</v>
+        <v>54</v>
       </c>
       <c r="K8" s="11"/>
       <c r="L8" s="11" t="s">
@@ -1408,22 +1488,22 @@
     </row>
     <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>103</v>
+        <v>57</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>104</v>
+        <v>58</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="D9" s="3" t="s">
         <v>16</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>105</v>
+        <v>57</v>
       </c>
       <c r="F9" s="3" t="s">
-        <v>106</v>
+        <v>58</v>
       </c>
       <c r="G9" s="3" t="s">
         <v>59</v>
@@ -1435,7 +1515,7 @@
         <v>18</v>
       </c>
       <c r="J9" s="3" t="s">
-        <v>107</v>
+        <v>61</v>
       </c>
       <c r="K9" s="11"/>
       <c r="L9" s="11" t="s">
@@ -1443,12 +1523,12 @@
       </c>
       <c r="M9" s="11"/>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
-        <v>119</v>
+        <v>55</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>120</v>
+        <v>56</v>
       </c>
       <c r="C10" s="3" t="s">
         <v>23</v>
@@ -1457,13 +1537,13 @@
         <v>16</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>121</v>
+        <v>57</v>
       </c>
       <c r="F10" s="3" t="s">
-        <v>122</v>
+        <v>58</v>
       </c>
       <c r="G10" s="3" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H10" s="3" t="s">
         <v>26</v>
@@ -1472,7 +1552,7 @@
         <v>27</v>
       </c>
       <c r="J10" s="3" t="s">
-        <v>123</v>
+        <v>60</v>
       </c>
       <c r="K10" s="11"/>
       <c r="L10" s="11" t="s">
@@ -1481,51 +1561,51 @@
       <c r="M10" s="11"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A11" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="B11" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="E11" s="3" t="s">
-        <v>151</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="G11" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="A11" s="12" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="12" t="s">
+        <v>121</v>
+      </c>
+      <c r="F11" s="12" t="s">
+        <v>122</v>
+      </c>
+      <c r="G11" s="12" t="s">
+        <v>23</v>
+      </c>
+      <c r="H11" s="12" t="s">
         <v>26</v>
       </c>
-      <c r="I11" s="3" t="s">
+      <c r="I11" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="J11" s="3" t="s">
-        <v>153</v>
-      </c>
-      <c r="K11" s="11"/>
-      <c r="L11" s="11" t="s">
+      <c r="J11" s="12" t="s">
+        <v>123</v>
+      </c>
+      <c r="K11" s="13"/>
+      <c r="L11" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="M11" s="11"/>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" s="17" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
-        <v>74</v>
+        <v>100</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>75</v>
+        <v>101</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D12" s="2" t="s">
         <v>16</v>
@@ -1540,202 +1620,204 @@
         <v>18</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>77</v>
+        <v>102</v>
       </c>
       <c r="K12" s="11"/>
       <c r="L12" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="M12" s="11"/>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="M12" s="11" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="B13" s="15" t="s">
+        <v>163</v>
+      </c>
+      <c r="C13" s="15" t="s">
+        <v>72</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E13" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F13" s="15" t="s">
+        <v>111</v>
+      </c>
+      <c r="G13" s="15" t="s">
+        <v>59</v>
+      </c>
+      <c r="H13" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I13" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J13" s="15" t="s">
+        <v>164</v>
+      </c>
+      <c r="K13" s="16"/>
+      <c r="L13" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M13" s="16" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="15" t="s">
+        <v>74</v>
+      </c>
+      <c r="B14" s="15" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="15"/>
+      <c r="G14" s="15"/>
+      <c r="H14" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J14" s="15" t="s">
+        <v>77</v>
+      </c>
+      <c r="K14" s="16"/>
+      <c r="L14" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M14" s="16" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A15" s="15" t="s">
+        <v>86</v>
+      </c>
+      <c r="B15" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="C15" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="15"/>
+      <c r="G15" s="15"/>
+      <c r="H15" s="15" t="s">
+        <v>76</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>18</v>
+      </c>
+      <c r="J15" s="15" t="s">
+        <v>88</v>
+      </c>
+      <c r="K15" s="16"/>
+      <c r="L15" s="16" t="s">
+        <v>20</v>
+      </c>
+      <c r="M15" s="16"/>
+    </row>
+    <row r="16" spans="1:13" s="17" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="15" t="s">
         <v>83</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B16" s="15" t="s">
         <v>84</v>
       </c>
-      <c r="C13" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D13" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E13" s="2"/>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2" t="s">
+      <c r="C16" s="15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+      <c r="G16" s="15"/>
+      <c r="H16" s="15" t="s">
         <v>76</v>
       </c>
-      <c r="I13" s="2" t="s">
+      <c r="I16" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J13" s="2" t="s">
+      <c r="J16" s="15" t="s">
         <v>85</v>
       </c>
-      <c r="K13" s="11"/>
-      <c r="L13" s="11" t="s">
+      <c r="K16" s="16"/>
+      <c r="L16" s="16" t="s">
         <v>20</v>
       </c>
-      <c r="M13" s="11"/>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A14" s="2" t="s">
-        <v>86</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>87</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D14" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J14" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="K14" s="11"/>
-      <c r="L14" s="11" t="s">
+      <c r="M16" s="16"/>
+    </row>
+    <row r="17" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="18" t="s">
+        <v>94</v>
+      </c>
+      <c r="B17" s="18" t="s">
+        <v>95</v>
+      </c>
+      <c r="C17" s="18" t="s">
+        <v>96</v>
+      </c>
+      <c r="D17" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E17" s="18" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="18" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H17" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I17" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J17" s="18" t="s">
+        <v>99</v>
+      </c>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M14" s="11"/>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A15" s="2" t="s">
-        <v>100</v>
-      </c>
-      <c r="B15" s="2" t="s">
-        <v>101</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="M17" s="13"/>
+    </row>
+    <row r="18" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="4"/>
+      <c r="F18" s="4"/>
+      <c r="G18" s="4" t="s">
         <v>59</v>
-      </c>
-      <c r="D15" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I15" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J15" s="2" t="s">
-        <v>102</v>
-      </c>
-      <c r="K15" s="11"/>
-      <c r="L15" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M15" s="11"/>
-    </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A16" s="2" t="s">
-        <v>162</v>
-      </c>
-      <c r="B16" s="2" t="s">
-        <v>163</v>
-      </c>
-      <c r="C16" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D16" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>110</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>111</v>
-      </c>
-      <c r="G16" s="2" t="s">
-        <v>59</v>
-      </c>
-      <c r="H16" s="2" t="s">
-        <v>76</v>
-      </c>
-      <c r="I16" s="2" t="s">
-        <v>18</v>
-      </c>
-      <c r="J16" s="2" t="s">
-        <v>164</v>
-      </c>
-      <c r="K16" s="11"/>
-      <c r="L16" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M16" s="11"/>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A17" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D17" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E17" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="F17" s="4" t="s">
-        <v>36</v>
-      </c>
-      <c r="G17" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H17" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I17" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="J17" s="4" t="s">
-        <v>38</v>
-      </c>
-      <c r="K17" s="11"/>
-      <c r="L17" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M17" s="11"/>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A18" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D18" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E18" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="F18" s="4" t="s">
-        <v>68</v>
-      </c>
-      <c r="G18" s="4" t="s">
-        <v>23</v>
       </c>
       <c r="H18" s="4" t="s">
         <v>37</v>
@@ -1744,44 +1826,48 @@
         <v>18</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>69</v>
-      </c>
-      <c r="K18" s="11"/>
+        <v>112</v>
+      </c>
+      <c r="K18" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="L18" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="M18" s="11"/>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="M18" s="11" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19" s="4" t="s">
-        <v>78</v>
+        <v>116</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>79</v>
+        <v>117</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D19" s="4" t="s">
         <v>16</v>
       </c>
       <c r="E19" s="4" t="s">
-        <v>80</v>
+        <v>110</v>
       </c>
       <c r="F19" s="4" t="s">
-        <v>81</v>
+        <v>111</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="H19" s="4" t="s">
         <v>37</v>
       </c>
       <c r="I19" s="4" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>82</v>
+        <v>118</v>
       </c>
       <c r="K19" s="11"/>
       <c r="L19" s="11" t="s">
@@ -1790,48 +1876,48 @@
       <c r="M19" s="11"/>
     </row>
     <row r="20" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A20" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>96</v>
-      </c>
-      <c r="D20" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E20" s="4" t="s">
-        <v>97</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>98</v>
-      </c>
-      <c r="G20" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H20" s="4" t="s">
+      <c r="A20" s="18" t="s">
+        <v>33</v>
+      </c>
+      <c r="B20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="C20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D20" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E20" s="18" t="s">
+        <v>35</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>36</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H20" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="J20" s="4" t="s">
-        <v>99</v>
-      </c>
-      <c r="K20" s="11"/>
-      <c r="L20" s="11" t="s">
+      <c r="J20" s="18" t="s">
+        <v>38</v>
+      </c>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M20" s="11"/>
+      <c r="M20" s="13"/>
     </row>
     <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" s="4" t="s">
-        <v>108</v>
+        <v>174</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>109</v>
+        <v>175</v>
       </c>
       <c r="C21" s="4" t="s">
         <v>23</v>
@@ -1840,22 +1926,22 @@
         <v>16</v>
       </c>
       <c r="E21" s="4" t="s">
-        <v>110</v>
+        <v>24</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>111</v>
+        <v>25</v>
       </c>
       <c r="G21" s="4" t="s">
-        <v>59</v>
+        <v>23</v>
       </c>
       <c r="H21" s="4" t="s">
         <v>37</v>
       </c>
       <c r="I21" s="4" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J21" s="4" t="s">
-        <v>112</v>
+        <v>176</v>
       </c>
       <c r="K21" s="11"/>
       <c r="L21" s="11" t="s">
@@ -1865,10 +1951,10 @@
     </row>
     <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" s="4" t="s">
-        <v>113</v>
+        <v>154</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>114</v>
+        <v>120</v>
       </c>
       <c r="C22" s="4" t="s">
         <v>23</v>
@@ -1877,10 +1963,10 @@
         <v>16</v>
       </c>
       <c r="E22" s="4" t="s">
-        <v>67</v>
+        <v>41</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>68</v>
+        <v>42</v>
       </c>
       <c r="G22" s="4" t="s">
         <v>23</v>
@@ -1892,7 +1978,7 @@
         <v>18</v>
       </c>
       <c r="J22" s="4" t="s">
-        <v>115</v>
+        <v>155</v>
       </c>
       <c r="K22" s="11"/>
       <c r="L22" s="11" t="s">
@@ -1900,321 +1986,321 @@
       </c>
       <c r="M22" s="11"/>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A23" s="4" t="s">
-        <v>116</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>117</v>
-      </c>
-      <c r="C23" s="4" t="s">
+    <row r="23" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="18" t="s">
+        <v>165</v>
+      </c>
+      <c r="B23" s="18" t="s">
+        <v>166</v>
+      </c>
+      <c r="C23" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D23" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E23" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>111</v>
+      </c>
+      <c r="G23" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="D23" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F23" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G23" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H23" s="4" t="s">
+      <c r="H23" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I23" s="4" t="s">
+      <c r="I23" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J23" s="4" t="s">
-        <v>118</v>
-      </c>
-      <c r="K23" s="11"/>
-      <c r="L23" s="11" t="s">
+      <c r="J23" s="18" t="s">
+        <v>167</v>
+      </c>
+      <c r="K23" s="13"/>
+      <c r="L23" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M23" s="11"/>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A24" s="4" t="s">
-        <v>154</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>120</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D24" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="F24" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="G24" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H24" s="4" t="s">
+      <c r="M23" s="13"/>
+    </row>
+    <row r="24" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="18" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" s="18" t="s">
+        <v>114</v>
+      </c>
+      <c r="C24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D24" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G24" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H24" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I24" s="4" t="s">
+      <c r="I24" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J24" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="K24" s="11"/>
-      <c r="L24" s="11" t="s">
+      <c r="J24" s="18" t="s">
+        <v>115</v>
+      </c>
+      <c r="K24" s="13"/>
+      <c r="L24" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M24" s="11"/>
+      <c r="M24" s="13"/>
     </row>
     <row r="25" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A25" s="4" t="s">
-        <v>165</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>166</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D25" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="F25" s="4" t="s">
-        <v>111</v>
-      </c>
-      <c r="G25" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="H25" s="4" t="s">
+      <c r="A25" s="18" t="s">
+        <v>78</v>
+      </c>
+      <c r="B25" s="18" t="s">
+        <v>79</v>
+      </c>
+      <c r="C25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D25" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="18" t="s">
+        <v>80</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>81</v>
+      </c>
+      <c r="G25" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H25" s="18" t="s">
         <v>37</v>
       </c>
-      <c r="I25" s="4" t="s">
+      <c r="I25" s="18" t="s">
+        <v>27</v>
+      </c>
+      <c r="J25" s="18" t="s">
+        <v>82</v>
+      </c>
+      <c r="K25" s="13"/>
+      <c r="L25" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M25" s="13"/>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A26" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B26" s="18" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" s="18" t="s">
+        <v>16</v>
+      </c>
+      <c r="E26" s="18" t="s">
+        <v>67</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>68</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>23</v>
+      </c>
+      <c r="H26" s="18" t="s">
+        <v>37</v>
+      </c>
+      <c r="I26" s="18" t="s">
         <v>18</v>
       </c>
-      <c r="J25" s="4" t="s">
-        <v>167</v>
-      </c>
-      <c r="K25" s="11"/>
-      <c r="L25" s="11" t="s">
+      <c r="J26" s="18" t="s">
+        <v>69</v>
+      </c>
+      <c r="K26" s="13"/>
+      <c r="L26" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M25" s="11"/>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A26" s="4" t="s">
-        <v>174</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>175</v>
-      </c>
-      <c r="C26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="D26" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H26" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="I26" s="4" t="s">
+      <c r="M26" s="13"/>
+    </row>
+    <row r="27" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="20" t="s">
+        <v>168</v>
+      </c>
+      <c r="B27" s="20" t="s">
+        <v>169</v>
+      </c>
+      <c r="C27" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E27" s="20"/>
+      <c r="F27" s="20"/>
+      <c r="G27" s="20"/>
+      <c r="H27" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I27" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J26" s="4" t="s">
-        <v>176</v>
-      </c>
-      <c r="K26" s="11"/>
-      <c r="L26" s="11" t="s">
+      <c r="J27" s="20" t="s">
+        <v>170</v>
+      </c>
+      <c r="K27" s="13"/>
+      <c r="L27" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M26" s="11"/>
-    </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A27" s="2" t="s">
+      <c r="M27" s="13"/>
+    </row>
+    <row r="28" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="20" t="s">
         <v>13</v>
       </c>
-      <c r="B27" s="2" t="s">
+      <c r="B28" s="20" t="s">
         <v>14</v>
       </c>
-      <c r="C27" s="2" t="s">
+      <c r="C28" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="2"/>
-      <c r="F27" s="2"/>
-      <c r="G27" s="2"/>
-      <c r="H27" s="2" t="s">
+      <c r="D28" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="20"/>
+      <c r="H28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I27" s="2" t="s">
+      <c r="I28" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="J27" s="2" t="s">
+      <c r="J28" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="K27" s="11"/>
-      <c r="L27" s="11" t="s">
+      <c r="K28" s="13"/>
+      <c r="L28" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M27" s="11"/>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A28" s="2" t="s">
+      <c r="M28" s="13"/>
+    </row>
+    <row r="29" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>148</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>149</v>
+      </c>
+      <c r="C29" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D29" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E29" s="20"/>
+      <c r="F29" s="20"/>
+      <c r="G29" s="20"/>
+      <c r="H29" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="I29" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="J29" s="20" t="s">
+        <v>150</v>
+      </c>
+      <c r="K29" s="13"/>
+      <c r="L29" s="13" t="s">
+        <v>20</v>
+      </c>
+      <c r="M29" s="13"/>
+    </row>
+    <row r="30" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
         <v>30</v>
       </c>
-      <c r="B28" s="2" t="s">
+      <c r="B30" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="C28" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="2"/>
-      <c r="F28" s="2"/>
-      <c r="G28" s="2"/>
-      <c r="H28" s="2" t="s">
+      <c r="C30" s="20" t="s">
+        <v>23</v>
+      </c>
+      <c r="D30" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="E30" s="20"/>
+      <c r="F30" s="20"/>
+      <c r="G30" s="20"/>
+      <c r="H30" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I28" s="2" t="s">
+      <c r="I30" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J28" s="2" t="s">
+      <c r="J30" s="20" t="s">
         <v>32</v>
       </c>
-      <c r="K28" s="11"/>
-      <c r="L28" s="11" t="s">
+      <c r="K30" s="13"/>
+      <c r="L30" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M28" s="11"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A29" s="2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="2" t="s">
-        <v>23</v>
-      </c>
-      <c r="D29" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="2"/>
-      <c r="F29" s="2"/>
-      <c r="G29" s="2"/>
-      <c r="H29" s="2" t="s">
+      <c r="M30" s="13"/>
+    </row>
+    <row r="31" spans="1:13" s="14" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="20" t="s">
+        <v>127</v>
+      </c>
+      <c r="B31" s="20" t="s">
+        <v>128</v>
+      </c>
+      <c r="C31" s="20" t="s">
+        <v>129</v>
+      </c>
+      <c r="D31" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="E31" s="20"/>
+      <c r="F31" s="20"/>
+      <c r="G31" s="20"/>
+      <c r="H31" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="I29" s="2" t="s">
+      <c r="I31" s="20" t="s">
         <v>27</v>
       </c>
-      <c r="J29" s="2" t="s">
-        <v>64</v>
-      </c>
-      <c r="K29" s="11"/>
-      <c r="L29" s="11" t="s">
+      <c r="J31" s="20" t="s">
+        <v>130</v>
+      </c>
+      <c r="K31" s="13"/>
+      <c r="L31" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="M29" s="11"/>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A30" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="B30" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>72</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="2"/>
-      <c r="F30" s="2"/>
-      <c r="G30" s="2"/>
-      <c r="H30" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I30" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J30" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="K30" s="11"/>
-      <c r="L30" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M30" s="11"/>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
-      <c r="A31" s="2" t="s">
-        <v>124</v>
-      </c>
-      <c r="B31" s="2" t="s">
-        <v>125</v>
-      </c>
-      <c r="C31" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="D31" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="2"/>
-      <c r="F31" s="2"/>
-      <c r="G31" s="2"/>
-      <c r="H31" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="I31" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="J31" s="2" t="s">
-        <v>126</v>
-      </c>
-      <c r="K31" s="11"/>
-      <c r="L31" s="11" t="s">
-        <v>20</v>
-      </c>
-      <c r="M31" s="11"/>
+      <c r="M31" s="13"/>
     </row>
     <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" s="2" t="s">
-        <v>127</v>
+        <v>156</v>
       </c>
       <c r="B32" s="2" t="s">
-        <v>128</v>
+        <v>157</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>129</v>
+        <v>59</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
@@ -2223,26 +2309,28 @@
         <v>17</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>27</v>
+        <v>18</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>130</v>
+        <v>158</v>
       </c>
       <c r="K32" s="11"/>
       <c r="L32" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="M32" s="11"/>
+      <c r="M32" s="11" t="s">
+        <v>218</v>
+      </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" s="2" t="s">
-        <v>131</v>
+        <v>159</v>
       </c>
       <c r="B33" s="2" t="s">
-        <v>132</v>
+        <v>160</v>
       </c>
       <c r="C33" s="2" t="s">
-        <v>23</v>
+        <v>72</v>
       </c>
       <c r="D33" s="2" t="s">
         <v>16</v>
@@ -2257,7 +2345,7 @@
         <v>27</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>133</v>
+        <v>161</v>
       </c>
       <c r="K33" s="11"/>
       <c r="L33" s="11" t="s">
@@ -2267,13 +2355,13 @@
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" s="2" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="B34" s="2" t="s">
-        <v>135</v>
+        <v>132</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>96</v>
+        <v>23</v>
       </c>
       <c r="D34" s="2" t="s">
         <v>16</v>
@@ -2288,7 +2376,7 @@
         <v>27</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="K34" s="11"/>
       <c r="L34" s="11" t="s">
@@ -2298,13 +2386,13 @@
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" s="2" t="s">
-        <v>137</v>
+        <v>146</v>
       </c>
       <c r="B35" s="2" t="s">
-        <v>138</v>
+        <v>132</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>96</v>
+        <v>72</v>
       </c>
       <c r="D35" s="2" t="s">
         <v>16</v>
@@ -2319,7 +2407,7 @@
         <v>27</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>139</v>
+        <v>147</v>
       </c>
       <c r="K35" s="11"/>
       <c r="L35" s="11" t="s">
@@ -2329,10 +2417,10 @@
     </row>
     <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" s="2" t="s">
-        <v>140</v>
+        <v>134</v>
       </c>
       <c r="B36" s="2" t="s">
-        <v>141</v>
+        <v>135</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>96</v>
@@ -2350,7 +2438,7 @@
         <v>27</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>142</v>
+        <v>136</v>
       </c>
       <c r="K36" s="11"/>
       <c r="L36" s="11" t="s">
@@ -2360,13 +2448,13 @@
     </row>
     <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" s="2" t="s">
-        <v>143</v>
+        <v>137</v>
       </c>
       <c r="B37" s="2" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C37" s="2" t="s">
-        <v>59</v>
+        <v>96</v>
       </c>
       <c r="D37" s="2" t="s">
         <v>16</v>
@@ -2381,7 +2469,7 @@
         <v>27</v>
       </c>
       <c r="J37" s="2" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="K37" s="11"/>
       <c r="L37" s="11" t="s">
@@ -2391,13 +2479,13 @@
     </row>
     <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" s="2" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="B38" s="2" t="s">
-        <v>132</v>
+        <v>141</v>
       </c>
       <c r="C38" s="2" t="s">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="D38" s="2" t="s">
         <v>16</v>
@@ -2412,7 +2500,7 @@
         <v>27</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="K38" s="11"/>
       <c r="L38" s="11" t="s">
@@ -2422,13 +2510,13 @@
     </row>
     <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" s="2" t="s">
-        <v>148</v>
+        <v>143</v>
       </c>
       <c r="B39" s="2" t="s">
-        <v>149</v>
+        <v>144</v>
       </c>
       <c r="C39" s="2" t="s">
-        <v>23</v>
+        <v>59</v>
       </c>
       <c r="D39" s="2" t="s">
         <v>16</v>
@@ -2443,7 +2531,7 @@
         <v>27</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>150</v>
+        <v>145</v>
       </c>
       <c r="K39" s="11"/>
       <c r="L39" s="11" t="s">
@@ -2453,13 +2541,13 @@
     </row>
     <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" s="2" t="s">
-        <v>156</v>
+        <v>124</v>
       </c>
       <c r="B40" s="2" t="s">
-        <v>157</v>
+        <v>125</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>59</v>
+        <v>15</v>
       </c>
       <c r="D40" s="2" t="s">
         <v>16</v>
@@ -2471,10 +2559,10 @@
         <v>17</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>158</v>
+        <v>126</v>
       </c>
       <c r="K40" s="11"/>
       <c r="L40" s="11" t="s">
@@ -2484,13 +2572,13 @@
     </row>
     <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" s="2" t="s">
-        <v>159</v>
+        <v>62</v>
       </c>
       <c r="B41" s="2" t="s">
-        <v>160</v>
+        <v>63</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>72</v>
+        <v>23</v>
       </c>
       <c r="D41" s="2" t="s">
         <v>16</v>
@@ -2505,7 +2593,7 @@
         <v>27</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>161</v>
+        <v>64</v>
       </c>
       <c r="K41" s="11"/>
       <c r="L41" s="11" t="s">
@@ -2515,13 +2603,13 @@
     </row>
     <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" s="2" t="s">
-        <v>168</v>
+        <v>70</v>
       </c>
       <c r="B42" s="2" t="s">
-        <v>169</v>
+        <v>71</v>
       </c>
       <c r="C42" s="2" t="s">
-        <v>15</v>
+        <v>72</v>
       </c>
       <c r="D42" s="2" t="s">
         <v>16</v>
@@ -2536,7 +2624,7 @@
         <v>27</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>170</v>
+        <v>73</v>
       </c>
       <c r="K42" s="11"/>
       <c r="L42" s="11" t="s">
@@ -2575,9 +2663,23 @@
       </c>
       <c r="M43" s="11"/>
     </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A44" s="19" t="s">
+        <v>213</v>
+      </c>
+      <c r="B44" s="19"/>
+      <c r="C44" s="19"/>
+      <c r="D44" s="19"/>
+      <c r="E44" s="19"/>
+      <c r="F44" s="19"/>
+      <c r="G44" s="19"/>
+      <c r="H44" s="19"/>
+      <c r="I44" s="19"/>
+      <c r="J44" s="19"/>
+    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M43">
-    <sortCondition ref="H1:H43"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:M45">
+    <sortCondition ref="H1:H45"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>